<commit_message>
ci:update on ONCHO forms
</commit_message>
<xml_diff>
--- a/ONCHO/Breeding Site Survey/Cote d'Ivoire/civ_oncho_bsa_2_capture_form_202208.xlsx
+++ b/ONCHO/Breeding Site Survey/Cote d'Ivoire/civ_oncho_bsa_2_capture_form_202208.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="212">
   <si>
     <t>type</t>
   </si>
@@ -81,6 +81,15 @@
     <t>yes</t>
   </si>
   <si>
+    <t>select_one region</t>
+  </si>
+  <si>
+    <t>b_region</t>
+  </si>
+  <si>
+    <t>Sélectionner une région</t>
+  </si>
+  <si>
     <t>select_one district</t>
   </si>
   <si>
@@ -90,6 +99,9 @@
     <t>Sélectionner un district</t>
   </si>
   <si>
+    <t>region = ${b_region}</t>
+  </si>
+  <si>
     <t>string</t>
   </si>
   <si>
@@ -183,6 +195,9 @@
     <t>list_name</t>
   </si>
   <si>
+    <t>region</t>
+  </si>
+  <si>
     <t>district</t>
   </si>
   <si>
@@ -237,67 +252,385 @@
     <t>Ensoleillé</t>
   </si>
   <si>
-    <t>Agboville</t>
-  </si>
-  <si>
-    <t>Sikensi</t>
-  </si>
-  <si>
-    <t>Tiassalé</t>
-  </si>
-  <si>
-    <t>Koro</t>
-  </si>
-  <si>
-    <t>Ouaninou</t>
-  </si>
-  <si>
-    <t>Touba</t>
-  </si>
-  <si>
-    <t>Boundiali</t>
-  </si>
-  <si>
-    <t>Kouto</t>
-  </si>
-  <si>
-    <t>Didievi</t>
-  </si>
-  <si>
-    <t>Tiébissou</t>
-  </si>
-  <si>
-    <t>Toumodi</t>
-  </si>
-  <si>
-    <t>Yamoussoukro</t>
-  </si>
-  <si>
-    <t>Dianra</t>
-  </si>
-  <si>
-    <t>Kounahiri</t>
-  </si>
-  <si>
-    <t>Mankono</t>
-  </si>
-  <si>
-    <t>Bouna</t>
-  </si>
-  <si>
-    <t>Doropo</t>
-  </si>
-  <si>
-    <t>Nassian</t>
-  </si>
-  <si>
-    <t>Tehini</t>
-  </si>
-  <si>
-    <t>Blolequin</t>
-  </si>
-  <si>
-    <t>Guiglo</t>
+    <t>AGNEBY-TIASSA</t>
+  </si>
+  <si>
+    <t>BAFING</t>
+  </si>
+  <si>
+    <t>BAGOUE</t>
+  </si>
+  <si>
+    <t>BELIER</t>
+  </si>
+  <si>
+    <t>BERE</t>
+  </si>
+  <si>
+    <t>BOUKANI</t>
+  </si>
+  <si>
+    <t>CAVALLY</t>
+  </si>
+  <si>
+    <t>FOLON</t>
+  </si>
+  <si>
+    <t>GBEKE</t>
+  </si>
+  <si>
+    <t>GBOKLE</t>
+  </si>
+  <si>
+    <t>GOH</t>
+  </si>
+  <si>
+    <t>GONTOUGO</t>
+  </si>
+  <si>
+    <t>GRANDS PONTS</t>
+  </si>
+  <si>
+    <t>GUEMON</t>
+  </si>
+  <si>
+    <t>HAMBOL</t>
+  </si>
+  <si>
+    <t>HAUT SASSANDRA</t>
+  </si>
+  <si>
+    <t>IFFOU</t>
+  </si>
+  <si>
+    <t>INDENIE-DJUABLIN</t>
+  </si>
+  <si>
+    <t>KABADOUGOU</t>
+  </si>
+  <si>
+    <t>LOH-DJIBOUA</t>
+  </si>
+  <si>
+    <t>MARAHOUE</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>MORONOU</t>
+  </si>
+  <si>
+    <t>NAWA</t>
+  </si>
+  <si>
+    <t>N.ZI</t>
+  </si>
+  <si>
+    <t>N'ZI</t>
+  </si>
+  <si>
+    <t>PORO</t>
+  </si>
+  <si>
+    <t>SAN-PEDRO</t>
+  </si>
+  <si>
+    <t>SUD-COMOE</t>
+  </si>
+  <si>
+    <t>TCHOLOGO</t>
+  </si>
+  <si>
+    <t>TONKPI</t>
+  </si>
+  <si>
+    <t>WORODOUGOU</t>
+  </si>
+  <si>
+    <t>AGBOVILLE</t>
+  </si>
+  <si>
+    <t>SIKENSI</t>
+  </si>
+  <si>
+    <t>TIASSALE</t>
+  </si>
+  <si>
+    <t>KORO</t>
+  </si>
+  <si>
+    <t>OUANINOU</t>
+  </si>
+  <si>
+    <t>TOUBA</t>
+  </si>
+  <si>
+    <t>BOUNDIALI</t>
+  </si>
+  <si>
+    <t>KOUTO</t>
+  </si>
+  <si>
+    <t>DIDIEVI</t>
+  </si>
+  <si>
+    <t>TIEBISSOU</t>
+  </si>
+  <si>
+    <t>TOUMODI</t>
+  </si>
+  <si>
+    <t>YAMOUSSOUKRO</t>
+  </si>
+  <si>
+    <t>DIANRA</t>
+  </si>
+  <si>
+    <t>KOUNAHIRI</t>
+  </si>
+  <si>
+    <t>MANKONO</t>
+  </si>
+  <si>
+    <t>BOUNA</t>
+  </si>
+  <si>
+    <t>DOROPO</t>
+  </si>
+  <si>
+    <t>NASSIAN</t>
+  </si>
+  <si>
+    <t>TEHINI</t>
+  </si>
+  <si>
+    <t>BLOLEQUIN</t>
+  </si>
+  <si>
+    <t>GUIGLO</t>
+  </si>
+  <si>
+    <t>TAI</t>
+  </si>
+  <si>
+    <t>TOULEPLEU</t>
+  </si>
+  <si>
+    <t>KANIASSO</t>
+  </si>
+  <si>
+    <t>MINIGNAN</t>
+  </si>
+  <si>
+    <t>BEOUMI</t>
+  </si>
+  <si>
+    <t>BOTRO</t>
+  </si>
+  <si>
+    <t>BOUAKE NORD-EST</t>
+  </si>
+  <si>
+    <t>BOUAKE NORD-OUEST</t>
+  </si>
+  <si>
+    <t>SAKASSOU</t>
+  </si>
+  <si>
+    <t>FRESCO</t>
+  </si>
+  <si>
+    <t>SASSANDRA</t>
+  </si>
+  <si>
+    <t>GAGNOA 1</t>
+  </si>
+  <si>
+    <t>GAGNOA 2</t>
+  </si>
+  <si>
+    <t>OUME</t>
+  </si>
+  <si>
+    <t>BONDOUKOU</t>
+  </si>
+  <si>
+    <t>SANDEGUE</t>
+  </si>
+  <si>
+    <t>TANDA</t>
+  </si>
+  <si>
+    <t>DABOU</t>
+  </si>
+  <si>
+    <t>BANGOLO (3)</t>
+  </si>
+  <si>
+    <t>DUEKOUE (3)</t>
+  </si>
+  <si>
+    <t>KOUIBLY (1)</t>
+  </si>
+  <si>
+    <t>DABAKALA</t>
+  </si>
+  <si>
+    <t>KATIOLA</t>
+  </si>
+  <si>
+    <t>NIAKARA</t>
+  </si>
+  <si>
+    <t>DALOA</t>
+  </si>
+  <si>
+    <t>ISSIA</t>
+  </si>
+  <si>
+    <t>VAVOUA</t>
+  </si>
+  <si>
+    <t>ZOUKOUGBEU</t>
+  </si>
+  <si>
+    <t>DAOUKRO</t>
+  </si>
+  <si>
+    <t>M'BAHIAKRO</t>
+  </si>
+  <si>
+    <t>PRIKRO</t>
+  </si>
+  <si>
+    <t>ABENGOUROU</t>
+  </si>
+  <si>
+    <t>BETTIE</t>
+  </si>
+  <si>
+    <t>MADINANI</t>
+  </si>
+  <si>
+    <t>ODIENNE</t>
+  </si>
+  <si>
+    <t>DIVO</t>
+  </si>
+  <si>
+    <t>GUITRY</t>
+  </si>
+  <si>
+    <t>LAKOTA</t>
+  </si>
+  <si>
+    <t>BOUAFLE</t>
+  </si>
+  <si>
+    <t>SINFRA</t>
+  </si>
+  <si>
+    <t>ZUENOULA</t>
+  </si>
+  <si>
+    <t>ADZOPE</t>
+  </si>
+  <si>
+    <t>AKOUPE</t>
+  </si>
+  <si>
+    <t>ALEPE</t>
+  </si>
+  <si>
+    <t>YAKASSE-ATTOBROU</t>
+  </si>
+  <si>
+    <t>ARRAH</t>
+  </si>
+  <si>
+    <t>BONGOUANOU</t>
+  </si>
+  <si>
+    <t>M'BATTO</t>
+  </si>
+  <si>
+    <t>BUYO</t>
+  </si>
+  <si>
+    <t>GUEYO</t>
+  </si>
+  <si>
+    <t>MEAGUI</t>
+  </si>
+  <si>
+    <t>SOUBRE</t>
+  </si>
+  <si>
+    <t>BOCANDA</t>
+  </si>
+  <si>
+    <t>DIMBOKRO</t>
+  </si>
+  <si>
+    <t>KOUASSI-KOUASSIKRO</t>
+  </si>
+  <si>
+    <t>DIKOUDOUGOU</t>
+  </si>
+  <si>
+    <t>KORHOGO 1</t>
+  </si>
+  <si>
+    <t>KORHOGO 2</t>
+  </si>
+  <si>
+    <t>M'BENGUE</t>
+  </si>
+  <si>
+    <t>SINEMENTIALI</t>
+  </si>
+  <si>
+    <t>TABOU</t>
+  </si>
+  <si>
+    <t>ABOISSO</t>
+  </si>
+  <si>
+    <t>ADIAKE</t>
+  </si>
+  <si>
+    <t>GRAND-BASSAM</t>
+  </si>
+  <si>
+    <t>TIAPOUM</t>
+  </si>
+  <si>
+    <t>FERKESSEDOUGOU</t>
+  </si>
+  <si>
+    <t>KONG</t>
+  </si>
+  <si>
+    <t>OUANGOLODOUGOU</t>
+  </si>
+  <si>
+    <t>BIANKOUMA (3)</t>
+  </si>
+  <si>
+    <t>DANANE (2)</t>
+  </si>
+  <si>
+    <t>MAN (4)</t>
+  </si>
+  <si>
+    <t>ZOUAN-HOUNIEN (1)</t>
+  </si>
+  <si>
+    <t>KANI</t>
+  </si>
+  <si>
+    <t>SEGUELA</t>
   </si>
   <si>
     <t>form_title</t>
@@ -312,10 +645,10 @@
     <t>allow_choice_duplicates</t>
   </si>
   <si>
-    <t>(Août 2022) 2. Fiche de collecte des Simulies par équipe V2</t>
-  </si>
-  <si>
-    <t>civ_oncho_bsa_2_capture_form_202208_v2</t>
+    <t>(Août 2022) 2. Fiche de collecte des Simulies par équipe V3</t>
+  </si>
+  <si>
+    <t>civ_oncho_bsa_2_capture_form_202208_v3</t>
   </si>
   <si>
     <t>French</t>
@@ -327,9 +660,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -372,7 +705,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -393,10 +726,39 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -432,30 +794,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -469,17 +810,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -499,18 +831,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -529,13 +862,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -547,67 +940,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -625,19 +970,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -649,13 +982,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -667,49 +1030,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -738,6 +1071,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -747,11 +1095,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -771,17 +1125,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -812,21 +1160,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -838,142 +1171,142 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1363,10 +1696,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -1479,44 +1812,46 @@
       <c r="J3" s="18" t="s">
         <v>20</v>
       </c>
+      <c r="K3" s="3"/>
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
     </row>
-    <row r="4" s="3" customFormat="1" ht="15.75" customHeight="1" spans="1:13">
+    <row r="4" s="3" customFormat="1" spans="1:13">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
       <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
       <c r="J4" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="7"/>
-      <c r="M4" s="9"/>
+      <c r="L4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="10"/>
     </row>
     <row r="5" s="3" customFormat="1" ht="15.75" customHeight="1" spans="1:13">
       <c r="A5" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="9"/>
+        <v>30</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
@@ -1530,13 +1865,13 @@
     </row>
     <row r="6" s="3" customFormat="1" ht="15.75" customHeight="1" spans="1:13">
       <c r="A6" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -1552,13 +1887,13 @@
     </row>
     <row r="7" s="3" customFormat="1" ht="15.75" customHeight="1" spans="1:13">
       <c r="A7" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -1572,29 +1907,27 @@
       <c r="L7" s="7"/>
       <c r="M7" s="9"/>
     </row>
-    <row r="8" s="3" customFormat="1" spans="1:12">
-      <c r="A8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="12" t="s">
+    <row r="8" s="3" customFormat="1" ht="15.75" customHeight="1" spans="1:13">
+      <c r="A8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="B8" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7" t="s">
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="7"/>
       <c r="L8" s="7"/>
+      <c r="M8" s="9"/>
     </row>
     <row r="9" s="3" customFormat="1" spans="1:12">
       <c r="A9" s="6" t="s">
@@ -1606,10 +1939,10 @@
       <c r="C9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="7" t="s">
+      <c r="D9" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="E9" s="7"/>
       <c r="F9" s="6"/>
       <c r="G9" s="8"/>
       <c r="H9" s="7"/>
@@ -1622,16 +1955,18 @@
     </row>
     <row r="10" s="3" customFormat="1" spans="1:12">
       <c r="A10" s="6" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D10" s="8"/>
-      <c r="E10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="F10" s="6"/>
       <c r="G10" s="8"/>
       <c r="H10" s="7"/>
@@ -1644,13 +1979,13 @@
     </row>
     <row r="11" s="3" customFormat="1" spans="1:12">
       <c r="A11" s="6" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="7"/>
@@ -1666,48 +2001,52 @@
     </row>
     <row r="12" s="3" customFormat="1" spans="1:12">
       <c r="A12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
+      <c r="B12" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
     </row>
     <row r="13" s="3" customFormat="1" spans="1:12">
       <c r="A13" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="13"/>
+        <v>28</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>53</v>
+      </c>
       <c r="D13" s="13"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
     </row>
     <row r="14" s="3" customFormat="1" spans="1:12">
       <c r="A14" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -1721,8 +2060,12 @@
       <c r="L14" s="6"/>
     </row>
     <row r="15" s="3" customFormat="1" spans="1:12">
-      <c r="A15" s="6"/>
-      <c r="B15" s="14"/>
+      <c r="A15" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>57</v>
+      </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="6"/>
@@ -1734,10 +2077,19 @@
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
     </row>
-    <row r="16" s="3" customFormat="1" spans="2:4">
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
+    <row r="16" s="3" customFormat="1" spans="1:12">
+      <c r="A16" s="6"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
     </row>
     <row r="17" s="3" customFormat="1" spans="2:4">
       <c r="B17" s="9"/>
@@ -1745,9 +2097,14 @@
       <c r="D17" s="9"/>
     </row>
     <row r="18" s="3" customFormat="1" spans="2:4">
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" s="3" customFormat="1" spans="2:4">
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1759,24 +2116,24 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:F144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A82" sqref="$A82:$XFD123"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="16.3777777777778" customWidth="1"/>
     <col min="2" max="2" width="39.6222222222222" customWidth="1"/>
     <col min="3" max="3" width="13.1259259259259" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
@@ -1785,395 +2142,1852 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" t="s">
+        <v>104</v>
+      </c>
+      <c r="C42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" t="s">
+        <v>108</v>
+      </c>
+      <c r="C46" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" t="s">
+        <v>110</v>
+      </c>
+      <c r="C49" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" t="s">
+        <v>111</v>
+      </c>
+      <c r="D50" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51" t="s">
+        <v>112</v>
+      </c>
+      <c r="D51" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" t="s">
+        <v>113</v>
+      </c>
+      <c r="C52" t="s">
+        <v>113</v>
+      </c>
+      <c r="D52" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" t="s">
+        <v>114</v>
+      </c>
+      <c r="D53" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" t="s">
+        <v>115</v>
+      </c>
+      <c r="C54" t="s">
+        <v>115</v>
+      </c>
+      <c r="D54" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55" t="s">
+        <v>116</v>
+      </c>
+      <c r="C55" t="s">
+        <v>116</v>
+      </c>
+      <c r="D55" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" t="s">
+        <v>117</v>
+      </c>
+      <c r="C56" t="s">
+        <v>117</v>
+      </c>
+      <c r="D56" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57" t="s">
+        <v>118</v>
+      </c>
+      <c r="D57" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" t="s">
+        <v>119</v>
+      </c>
+      <c r="D58" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59" t="s">
+        <v>120</v>
+      </c>
+      <c r="D59" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" t="s">
+        <v>121</v>
+      </c>
+      <c r="D60" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" t="s">
+        <v>122</v>
+      </c>
+      <c r="D61" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>123</v>
+      </c>
+      <c r="C62" t="s">
+        <v>123</v>
+      </c>
+      <c r="D62" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" t="s">
+        <v>124</v>
+      </c>
+      <c r="C63" t="s">
+        <v>124</v>
+      </c>
+      <c r="D63" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>60</v>
+      </c>
+      <c r="B64" t="s">
+        <v>125</v>
+      </c>
+      <c r="C64" t="s">
+        <v>125</v>
+      </c>
+      <c r="D64" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>60</v>
+      </c>
+      <c r="B65" t="s">
+        <v>126</v>
+      </c>
+      <c r="C65" t="s">
+        <v>126</v>
+      </c>
+      <c r="D65" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>60</v>
+      </c>
+      <c r="B66" t="s">
+        <v>127</v>
+      </c>
+      <c r="C66" t="s">
+        <v>127</v>
+      </c>
+      <c r="D66" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
+        <v>60</v>
+      </c>
+      <c r="B67" t="s">
+        <v>128</v>
+      </c>
+      <c r="C67" t="s">
+        <v>128</v>
+      </c>
+      <c r="D67" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>60</v>
+      </c>
+      <c r="B68" t="s">
+        <v>129</v>
+      </c>
+      <c r="C68" t="s">
+        <v>129</v>
+      </c>
+      <c r="D68" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>60</v>
+      </c>
+      <c r="B69" t="s">
+        <v>130</v>
+      </c>
+      <c r="C69" t="s">
+        <v>130</v>
+      </c>
+      <c r="D69" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>60</v>
+      </c>
+      <c r="B70" t="s">
+        <v>131</v>
+      </c>
+      <c r="C70" t="s">
+        <v>131</v>
+      </c>
+      <c r="D70" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>60</v>
+      </c>
+      <c r="B71" t="s">
+        <v>132</v>
+      </c>
+      <c r="C71" t="s">
+        <v>132</v>
+      </c>
+      <c r="D71" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
+        <v>60</v>
+      </c>
+      <c r="B72" t="s">
+        <v>133</v>
+      </c>
+      <c r="C72" t="s">
+        <v>133</v>
+      </c>
+      <c r="D72" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
+        <v>60</v>
+      </c>
+      <c r="B73" t="s">
+        <v>134</v>
+      </c>
+      <c r="C73" t="s">
+        <v>134</v>
+      </c>
+      <c r="D73" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>60</v>
+      </c>
+      <c r="B74" t="s">
+        <v>135</v>
+      </c>
+      <c r="C74" t="s">
+        <v>135</v>
+      </c>
+      <c r="D74" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" t="s">
+        <v>60</v>
+      </c>
+      <c r="B75" t="s">
+        <v>136</v>
+      </c>
+      <c r="C75" t="s">
+        <v>136</v>
+      </c>
+      <c r="D75" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
+        <v>60</v>
+      </c>
+      <c r="B76" t="s">
+        <v>137</v>
+      </c>
+      <c r="C76" t="s">
+        <v>137</v>
+      </c>
+      <c r="D76" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
+        <v>60</v>
+      </c>
+      <c r="B77" t="s">
+        <v>138</v>
+      </c>
+      <c r="C77" t="s">
+        <v>138</v>
+      </c>
+      <c r="D77" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" t="s">
+        <v>60</v>
+      </c>
+      <c r="B78" t="s">
+        <v>139</v>
+      </c>
+      <c r="C78" t="s">
+        <v>139</v>
+      </c>
+      <c r="D78" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>60</v>
+      </c>
+      <c r="B79" t="s">
+        <v>140</v>
+      </c>
+      <c r="C79" t="s">
+        <v>140</v>
+      </c>
+      <c r="D79" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
+        <v>60</v>
+      </c>
+      <c r="B80" t="s">
+        <v>141</v>
+      </c>
+      <c r="C80" t="s">
+        <v>141</v>
+      </c>
+      <c r="D80" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" t="s">
+        <v>60</v>
+      </c>
+      <c r="B81" t="s">
+        <v>142</v>
+      </c>
+      <c r="C81" t="s">
+        <v>142</v>
+      </c>
+      <c r="D81" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" t="s">
+        <v>60</v>
+      </c>
+      <c r="B82" t="s">
+        <v>143</v>
+      </c>
+      <c r="C82" t="s">
+        <v>143</v>
+      </c>
+      <c r="D82" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" t="s">
+        <v>60</v>
+      </c>
+      <c r="B83" t="s">
+        <v>144</v>
+      </c>
+      <c r="C83" t="s">
+        <v>144</v>
+      </c>
+      <c r="D83" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" t="s">
+        <v>60</v>
+      </c>
+      <c r="B84" t="s">
+        <v>145</v>
+      </c>
+      <c r="C84" t="s">
+        <v>145</v>
+      </c>
+      <c r="D84" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" t="s">
+        <v>60</v>
+      </c>
+      <c r="B85" t="s">
+        <v>146</v>
+      </c>
+      <c r="C85" t="s">
+        <v>146</v>
+      </c>
+      <c r="D85" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" t="s">
+        <v>60</v>
+      </c>
+      <c r="B86" t="s">
+        <v>147</v>
+      </c>
+      <c r="C86" t="s">
+        <v>147</v>
+      </c>
+      <c r="D86" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" t="s">
+        <v>60</v>
+      </c>
+      <c r="B87" t="s">
+        <v>148</v>
+      </c>
+      <c r="C87" t="s">
+        <v>148</v>
+      </c>
+      <c r="D87" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" t="s">
+        <v>60</v>
+      </c>
+      <c r="B88" t="s">
+        <v>149</v>
+      </c>
+      <c r="C88" t="s">
+        <v>149</v>
+      </c>
+      <c r="D88" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" t="s">
+        <v>60</v>
+      </c>
+      <c r="B89" t="s">
+        <v>150</v>
+      </c>
+      <c r="C89" t="s">
+        <v>150</v>
+      </c>
+      <c r="D89" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" t="s">
+        <v>60</v>
+      </c>
+      <c r="B90" t="s">
+        <v>151</v>
+      </c>
+      <c r="C90" t="s">
+        <v>151</v>
+      </c>
+      <c r="D90" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" t="s">
+        <v>60</v>
+      </c>
+      <c r="B91" t="s">
+        <v>152</v>
+      </c>
+      <c r="C91" t="s">
+        <v>152</v>
+      </c>
+      <c r="D91" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" t="s">
+        <v>60</v>
+      </c>
+      <c r="B92" t="s">
+        <v>153</v>
+      </c>
+      <c r="C92" t="s">
+        <v>153</v>
+      </c>
+      <c r="D92" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" t="s">
+        <v>60</v>
+      </c>
+      <c r="B93" t="s">
+        <v>154</v>
+      </c>
+      <c r="C93" t="s">
+        <v>154</v>
+      </c>
+      <c r="D93" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" t="s">
+        <v>60</v>
+      </c>
+      <c r="B94" t="s">
+        <v>155</v>
+      </c>
+      <c r="C94" t="s">
+        <v>155</v>
+      </c>
+      <c r="D94" t="s">
         <v>93</v>
       </c>
-      <c r="C37" s="3" t="s">
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" t="s">
+        <v>60</v>
+      </c>
+      <c r="B95" t="s">
+        <v>156</v>
+      </c>
+      <c r="C95" t="s">
+        <v>156</v>
+      </c>
+      <c r="D95" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" t="s">
+        <v>60</v>
+      </c>
+      <c r="B96" t="s">
+        <v>157</v>
+      </c>
+      <c r="C96" t="s">
+        <v>157</v>
+      </c>
+      <c r="D96" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" t="s">
+        <v>60</v>
+      </c>
+      <c r="B97" t="s">
+        <v>158</v>
+      </c>
+      <c r="C97" t="s">
+        <v>158</v>
+      </c>
+      <c r="D97" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" t="s">
+        <v>60</v>
+      </c>
+      <c r="B98" t="s">
+        <v>159</v>
+      </c>
+      <c r="C98" t="s">
+        <v>159</v>
+      </c>
+      <c r="D98" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" t="s">
+        <v>60</v>
+      </c>
+      <c r="B99" t="s">
+        <v>160</v>
+      </c>
+      <c r="C99" t="s">
+        <v>160</v>
+      </c>
+      <c r="D99" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" t="s">
+        <v>60</v>
+      </c>
+      <c r="B100" t="s">
+        <v>161</v>
+      </c>
+      <c r="C100" t="s">
+        <v>161</v>
+      </c>
+      <c r="D100" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" t="s">
+        <v>60</v>
+      </c>
+      <c r="B101" t="s">
+        <v>162</v>
+      </c>
+      <c r="C101" t="s">
+        <v>162</v>
+      </c>
+      <c r="D101" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" t="s">
+        <v>60</v>
+      </c>
+      <c r="B102" t="s">
+        <v>163</v>
+      </c>
+      <c r="C102" t="s">
+        <v>163</v>
+      </c>
+      <c r="D102" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" t="s">
+        <v>60</v>
+      </c>
+      <c r="B103" t="s">
+        <v>164</v>
+      </c>
+      <c r="C103" t="s">
+        <v>164</v>
+      </c>
+      <c r="D103" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" t="s">
+        <v>60</v>
+      </c>
+      <c r="B104" t="s">
+        <v>165</v>
+      </c>
+      <c r="C104" t="s">
+        <v>165</v>
+      </c>
+      <c r="D104" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" t="s">
+        <v>60</v>
+      </c>
+      <c r="B105" t="s">
+        <v>166</v>
+      </c>
+      <c r="C105" t="s">
+        <v>166</v>
+      </c>
+      <c r="D105" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" t="s">
+        <v>60</v>
+      </c>
+      <c r="B106" t="s">
+        <v>167</v>
+      </c>
+      <c r="C106" t="s">
+        <v>167</v>
+      </c>
+      <c r="D106" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" t="s">
+        <v>60</v>
+      </c>
+      <c r="B107" t="s">
+        <v>168</v>
+      </c>
+      <c r="C107" t="s">
+        <v>168</v>
+      </c>
+      <c r="D107" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" t="s">
+        <v>60</v>
+      </c>
+      <c r="B108" t="s">
+        <v>169</v>
+      </c>
+      <c r="C108" t="s">
+        <v>169</v>
+      </c>
+      <c r="D108" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" t="s">
+        <v>60</v>
+      </c>
+      <c r="B109" t="s">
+        <v>170</v>
+      </c>
+      <c r="C109" t="s">
+        <v>170</v>
+      </c>
+      <c r="D109" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" t="s">
+        <v>60</v>
+      </c>
+      <c r="B110" t="s">
+        <v>171</v>
+      </c>
+      <c r="C110" t="s">
+        <v>171</v>
+      </c>
+      <c r="D110" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" t="s">
+        <v>60</v>
+      </c>
+      <c r="B111" t="s">
+        <v>172</v>
+      </c>
+      <c r="C111" t="s">
+        <v>172</v>
+      </c>
+      <c r="D111" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" t="s">
+        <v>60</v>
+      </c>
+      <c r="B112" t="s">
+        <v>173</v>
+      </c>
+      <c r="C112" t="s">
+        <v>173</v>
+      </c>
+      <c r="D112" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" t="s">
+        <v>60</v>
+      </c>
+      <c r="B113" t="s">
+        <v>174</v>
+      </c>
+      <c r="C113" t="s">
+        <v>174</v>
+      </c>
+      <c r="D113" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" t="s">
+        <v>60</v>
+      </c>
+      <c r="B114" t="s">
+        <v>175</v>
+      </c>
+      <c r="C114" t="s">
+        <v>175</v>
+      </c>
+      <c r="D114" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" t="s">
+        <v>60</v>
+      </c>
+      <c r="B115" t="s">
+        <v>176</v>
+      </c>
+      <c r="C115" t="s">
+        <v>176</v>
+      </c>
+      <c r="D115" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" t="s">
+        <v>60</v>
+      </c>
+      <c r="B116" t="s">
+        <v>177</v>
+      </c>
+      <c r="C116" t="s">
+        <v>177</v>
+      </c>
+      <c r="D116" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" t="s">
+        <v>60</v>
+      </c>
+      <c r="B117" t="s">
+        <v>178</v>
+      </c>
+      <c r="C117" t="s">
+        <v>178</v>
+      </c>
+      <c r="D117" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" t="s">
+        <v>60</v>
+      </c>
+      <c r="B118" t="s">
+        <v>179</v>
+      </c>
+      <c r="C118" t="s">
+        <v>179</v>
+      </c>
+      <c r="D118" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" t="s">
+        <v>60</v>
+      </c>
+      <c r="B119" t="s">
+        <v>180</v>
+      </c>
+      <c r="C119" t="s">
+        <v>180</v>
+      </c>
+      <c r="D119" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" t="s">
+        <v>60</v>
+      </c>
+      <c r="B120" t="s">
+        <v>181</v>
+      </c>
+      <c r="C120" t="s">
+        <v>181</v>
+      </c>
+      <c r="D120" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" t="s">
+        <v>60</v>
+      </c>
+      <c r="B121" t="s">
+        <v>182</v>
+      </c>
+      <c r="C121" t="s">
+        <v>182</v>
+      </c>
+      <c r="D121" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" t="s">
+        <v>60</v>
+      </c>
+      <c r="B122" t="s">
+        <v>183</v>
+      </c>
+      <c r="C122" t="s">
+        <v>183</v>
+      </c>
+      <c r="D122" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" t="s">
+        <v>60</v>
+      </c>
+      <c r="B123" t="s">
+        <v>184</v>
+      </c>
+      <c r="C123" t="s">
+        <v>184</v>
+      </c>
+      <c r="D123" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" t="s">
+        <v>60</v>
+      </c>
+      <c r="B124" t="s">
+        <v>185</v>
+      </c>
+      <c r="C124" t="s">
+        <v>185</v>
+      </c>
+      <c r="D124" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" t="s">
+        <v>60</v>
+      </c>
+      <c r="B125" t="s">
+        <v>186</v>
+      </c>
+      <c r="C125" t="s">
+        <v>186</v>
+      </c>
+      <c r="D125" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" t="s">
+        <v>60</v>
+      </c>
+      <c r="B126" t="s">
+        <v>187</v>
+      </c>
+      <c r="C126" t="s">
+        <v>187</v>
+      </c>
+      <c r="D126" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" t="s">
+        <v>60</v>
+      </c>
+      <c r="B127" t="s">
+        <v>188</v>
+      </c>
+      <c r="C127" t="s">
+        <v>188</v>
+      </c>
+      <c r="D127" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" t="s">
+        <v>60</v>
+      </c>
+      <c r="B128" t="s">
+        <v>189</v>
+      </c>
+      <c r="C128" t="s">
+        <v>189</v>
+      </c>
+      <c r="D128" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" t="s">
+        <v>60</v>
+      </c>
+      <c r="B129" t="s">
+        <v>190</v>
+      </c>
+      <c r="C129" t="s">
+        <v>190</v>
+      </c>
+      <c r="D129" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" t="s">
+        <v>60</v>
+      </c>
+      <c r="B130" t="s">
+        <v>105</v>
+      </c>
+      <c r="C130" t="s">
+        <v>105</v>
+      </c>
+      <c r="D130" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" t="s">
+        <v>60</v>
+      </c>
+      <c r="B131" t="s">
+        <v>191</v>
+      </c>
+      <c r="C131" t="s">
+        <v>191</v>
+      </c>
+      <c r="D131" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" t="s">
+        <v>60</v>
+      </c>
+      <c r="B132" t="s">
+        <v>192</v>
+      </c>
+      <c r="C132" t="s">
+        <v>192</v>
+      </c>
+      <c r="D132" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" t="s">
+        <v>60</v>
+      </c>
+      <c r="B133" t="s">
+        <v>193</v>
+      </c>
+      <c r="C133" t="s">
+        <v>193</v>
+      </c>
+      <c r="D133" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" t="s">
+        <v>60</v>
+      </c>
+      <c r="B134" t="s">
+        <v>194</v>
+      </c>
+      <c r="C134" t="s">
+        <v>194</v>
+      </c>
+      <c r="D134" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" t="s">
+        <v>60</v>
+      </c>
+      <c r="B135" t="s">
+        <v>195</v>
+      </c>
+      <c r="C135" t="s">
+        <v>195</v>
+      </c>
+      <c r="D135" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" t="s">
+        <v>60</v>
+      </c>
+      <c r="B136" t="s">
+        <v>196</v>
+      </c>
+      <c r="C136" t="s">
+        <v>196</v>
+      </c>
+      <c r="D136" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" t="s">
+        <v>60</v>
+      </c>
+      <c r="B137" t="s">
+        <v>197</v>
+      </c>
+      <c r="C137" t="s">
+        <v>197</v>
+      </c>
+      <c r="D137" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" t="s">
+        <v>60</v>
+      </c>
+      <c r="B138" t="s">
+        <v>198</v>
+      </c>
+      <c r="C138" t="s">
+        <v>198</v>
+      </c>
+      <c r="D138" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" t="s">
+        <v>60</v>
+      </c>
+      <c r="B139" t="s">
+        <v>199</v>
+      </c>
+      <c r="C139" t="s">
+        <v>199</v>
+      </c>
+      <c r="D139" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" t="s">
+        <v>60</v>
+      </c>
+      <c r="B140" t="s">
+        <v>200</v>
+      </c>
+      <c r="C140" t="s">
+        <v>200</v>
+      </c>
+      <c r="D140" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" t="s">
+        <v>60</v>
+      </c>
+      <c r="B141" t="s">
+        <v>201</v>
+      </c>
+      <c r="C141" t="s">
+        <v>201</v>
+      </c>
+      <c r="D141" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" t="s">
+        <v>60</v>
+      </c>
+      <c r="B142" t="s">
+        <v>202</v>
+      </c>
+      <c r="C142" t="s">
+        <v>202</v>
+      </c>
+      <c r="D142" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" t="s">
+        <v>60</v>
+      </c>
+      <c r="B143" t="s">
+        <v>203</v>
+      </c>
+      <c r="C143" t="s">
+        <v>203</v>
+      </c>
+      <c r="D143" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" t="s">
+        <v>60</v>
+      </c>
+      <c r="B144" t="s">
+        <v>204</v>
+      </c>
+      <c r="C144" t="s">
+        <v>204</v>
+      </c>
+      <c r="D144" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2192,7 +4006,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -2203,27 +4017,27 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>205</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>95</v>
+        <v>206</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>96</v>
+        <v>207</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>97</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>98</v>
+        <v>209</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>210</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>211</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>

</xml_diff>